<commit_message>
Asservissement - doc to establish transfert function
</commit_message>
<xml_diff>
--- a/Documents/g.xlsx
+++ b/Documents/g.xlsx
@@ -402,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:K35"/>
+  <dimension ref="B4:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,22 +415,22 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <f>2^B4</f>
+        <f t="shared" ref="D4:D24" si="0">2^B4</f>
         <v>1</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
       </c>
       <c r="H4">
-        <f>SUM(D4:D23)</f>
-        <v>1048575</v>
+        <f>SUM(D4:D22)</f>
+        <v>524287</v>
       </c>
       <c r="J4" t="s">
         <v>14</v>
       </c>
       <c r="K4">
         <f>H4-H5</f>
-        <v>1048575</v>
+        <v>524287</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -438,7 +438,7 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <f>2^B5</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G5" t="s">
@@ -453,7 +453,7 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <f>2^B6</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -462,22 +462,22 @@
         <v>3</v>
       </c>
       <c r="D7">
-        <f>2^B7</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H7">
-        <f>SUM(D4:D24)</f>
-        <v>2097151</v>
+        <f>SUM(D4:D23)</f>
+        <v>1048575</v>
       </c>
       <c r="J7" t="s">
         <v>14</v>
       </c>
       <c r="K7">
-        <f t="shared" ref="K7" si="0">H7-H8</f>
-        <v>1048575</v>
+        <f t="shared" ref="K7" si="1">H7-H8</f>
+        <v>524287</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
@@ -485,15 +485,15 @@
         <v>4</v>
       </c>
       <c r="D8">
-        <f>2^B8</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H8" s="1">
         <f>H4+1</f>
-        <v>1048576</v>
+        <v>524288</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
@@ -501,7 +501,7 @@
         <v>5</v>
       </c>
       <c r="D9">
-        <f>2^B9</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
     </row>
@@ -510,7 +510,7 @@
         <v>6</v>
       </c>
       <c r="D10">
-        <f>2^B10</f>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
     </row>
@@ -519,7 +519,7 @@
         <v>7</v>
       </c>
       <c r="D11">
-        <f>2^B11</f>
+        <f t="shared" si="0"/>
         <v>128</v>
       </c>
       <c r="G11" t="s">
@@ -534,7 +534,7 @@
         <v>8</v>
       </c>
       <c r="D12">
-        <f>2^B12</f>
+        <f t="shared" si="0"/>
         <v>256</v>
       </c>
       <c r="G12" t="s">
@@ -549,7 +549,7 @@
         <v>9</v>
       </c>
       <c r="D13">
-        <f>2^B13</f>
+        <f t="shared" si="0"/>
         <v>512</v>
       </c>
       <c r="G13" t="s">
@@ -564,7 +564,7 @@
         <v>10</v>
       </c>
       <c r="D14">
-        <f>2^B14</f>
+        <f t="shared" si="0"/>
         <v>1024</v>
       </c>
       <c r="G14" t="s">
@@ -579,7 +579,7 @@
         <v>11</v>
       </c>
       <c r="D15">
-        <f>2^B15</f>
+        <f t="shared" si="0"/>
         <v>2048</v>
       </c>
     </row>
@@ -588,7 +588,7 @@
         <v>12</v>
       </c>
       <c r="D16">
-        <f>2^B16</f>
+        <f t="shared" si="0"/>
         <v>4096</v>
       </c>
     </row>
@@ -597,7 +597,7 @@
         <v>13</v>
       </c>
       <c r="D17">
-        <f>2^B17</f>
+        <f t="shared" si="0"/>
         <v>8192</v>
       </c>
     </row>
@@ -606,7 +606,7 @@
         <v>14</v>
       </c>
       <c r="D18">
-        <f>2^B18</f>
+        <f t="shared" si="0"/>
         <v>16384</v>
       </c>
     </row>
@@ -615,7 +615,7 @@
         <v>15</v>
       </c>
       <c r="D19">
-        <f>2^B19</f>
+        <f t="shared" si="0"/>
         <v>32768</v>
       </c>
     </row>
@@ -624,12 +624,11 @@
         <v>16</v>
       </c>
       <c r="D20">
-        <f>2^B20</f>
+        <f t="shared" si="0"/>
         <v>65536</v>
       </c>
       <c r="G20">
-        <f>SUM(D4:D23)</f>
-        <v>1048575</v>
+        <v>524287</v>
       </c>
       <c r="H20" s="1">
         <f>(G20-$H$5)*($H$11-$H$12)/($H$4-$H$5)+$H$12</f>
@@ -647,15 +646,15 @@
         <v>17</v>
       </c>
       <c r="D21">
-        <f>2^B21</f>
+        <f t="shared" si="0"/>
         <v>131072</v>
       </c>
       <c r="G21">
-        <v>800000</v>
+        <v>400000</v>
       </c>
       <c r="H21" s="1">
-        <f>(G21-$H$5)*($H$11-$H$12)/($H$4-$H$5)+$H$12</f>
-        <v>57767.260901699927</v>
+        <f t="shared" ref="H21:H26" si="2">(G21-$H$5)*($H$11-$H$12)/($H$4-$H$5)+$H$12</f>
+        <v>57767.284742898453</v>
       </c>
       <c r="J21" s="2"/>
     </row>
@@ -664,15 +663,15 @@
         <v>18</v>
       </c>
       <c r="D22">
-        <f>2^B22</f>
+        <f t="shared" si="0"/>
         <v>262144</v>
       </c>
       <c r="G22">
-        <v>600000</v>
+        <v>300000</v>
       </c>
       <c r="H22" s="1">
-        <f>(G22-$H$5)*($H$11-$H$12)/($H$4-$H$5)+$H$12</f>
-        <v>51517.445676274947</v>
+        <f t="shared" si="2"/>
+        <v>51517.463557173833</v>
       </c>
       <c r="J22" s="2"/>
     </row>
@@ -681,32 +680,25 @@
         <v>19</v>
       </c>
       <c r="D23">
-        <f>2^B23</f>
+        <f t="shared" si="0"/>
         <v>524288</v>
       </c>
       <c r="G23">
-        <v>400000</v>
+        <v>250000</v>
       </c>
       <c r="H23" s="1">
-        <f>(G23-$H$5)*($H$11-$H$12)/($H$4-$H$5)+$H$12</f>
-        <v>45267.63045084996</v>
+        <f t="shared" si="2"/>
+        <v>48392.55296431153</v>
       </c>
       <c r="J23" s="2"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <v>20</v>
-      </c>
-      <c r="D24">
-        <f>2^B24</f>
-        <v>1048576</v>
-      </c>
       <c r="G24">
         <v>200000</v>
       </c>
       <c r="H24" s="1">
-        <f>(G24-$H$5)*($H$11-$H$12)/($H$4-$H$5)+$H$12</f>
-        <v>39017.81522542498</v>
+        <f t="shared" si="2"/>
+        <v>45267.642371449227</v>
       </c>
       <c r="J24" s="2"/>
     </row>
@@ -715,8 +707,8 @@
         <v>100000</v>
       </c>
       <c r="H25" s="1">
-        <f>(G25-$H$5)*($H$11-$H$12)/($H$4-$H$5)+$H$12</f>
-        <v>35892.907612712494</v>
+        <f t="shared" si="2"/>
+        <v>39017.821185724613</v>
       </c>
       <c r="J25" s="2"/>
     </row>
@@ -725,8 +717,8 @@
         <v>50000</v>
       </c>
       <c r="H26" s="1">
-        <f>(G26-$H$5)*($H$11-$H$12)/($H$4-$H$5)+$H$12</f>
-        <v>34330.453806356243</v>
+        <f t="shared" si="2"/>
+        <v>35892.910592862303</v>
       </c>
       <c r="J26" s="2"/>
     </row>
@@ -748,11 +740,11 @@
         <v>13</v>
       </c>
       <c r="D28">
-        <f>SUM(D4:D24)</f>
-        <v>2097151</v>
+        <f>SUM(D4:D23)</f>
+        <v>1048575</v>
       </c>
       <c r="G28" s="1">
-        <v>1048576</v>
+        <v>524288</v>
       </c>
       <c r="H28" s="1">
         <f>(G28-$H$7)*($H$13-$H$14)/($H$8-$H$7)+$H$14</f>
@@ -762,74 +754,71 @@
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G29">
-        <v>1100000</v>
+        <v>600000</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" ref="H29:H34" si="1">(G29-$H$7)*($H$13-$H$14)/($H$8-$H$7)+$H$14</f>
-        <v>31160.047509238728</v>
+        <f>(G29-$H$7)*($H$13-$H$14)/($H$8-$H$7)+$H$14</f>
+        <v>28035.135383864181</v>
       </c>
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D30">
-        <f>SUM(D4:D23)</f>
-        <v>1048575</v>
+        <f>SUM(D4:D22)</f>
+        <v>524287</v>
       </c>
       <c r="G30">
-        <v>1200000</v>
+        <v>700000</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" si="1"/>
-        <v>28035.139896526238</v>
+        <f t="shared" ref="H29:H34" si="3">(G30-$H$7)*($H$13-$H$14)/($H$8-$H$7)+$H$14</f>
+        <v>21785.314198139567</v>
       </c>
       <c r="J30" s="2"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G31">
-        <v>1400000</v>
+        <v>750000</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="1"/>
-        <v>21785.324671101258</v>
+        <f t="shared" si="3"/>
+        <v>18660.403605277261</v>
       </c>
       <c r="J31" s="2"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G32">
-        <v>1600000</v>
+        <v>800000</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="1"/>
-        <v>15535.509445676274</v>
+        <f t="shared" si="3"/>
+        <v>15535.493012414956</v>
       </c>
       <c r="J32" s="2"/>
     </row>
     <row r="33" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G33">
-        <v>1800000</v>
+        <v>900000</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="1"/>
-        <v>9285.6942202512928</v>
+        <f t="shared" si="3"/>
+        <v>9285.6718266903426</v>
       </c>
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G34">
-        <v>2097151</v>
+        <v>1048575</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J34" s="2"/>
-    </row>
-    <row r="35" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="I35">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I34">
         <f>-8</f>
         <v>-8</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="J34" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -926,7 +915,7 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <f>(B9-$F$2)*($C$2-$C$3)/($F$3-$F$2)+$C$3</f>
+        <f t="shared" ref="C9:C16" si="0">(B9-$F$2)*($C$2-$C$3)/($F$3-$F$2)+$C$3</f>
         <v>65535</v>
       </c>
     </row>
@@ -935,7 +924,7 @@
         <v>6</v>
       </c>
       <c r="C10">
-        <f>(B10-$F$2)*($C$2-$C$3)/($F$3-$F$2)+$C$3</f>
+        <f t="shared" si="0"/>
         <v>60854</v>
       </c>
     </row>
@@ -944,7 +933,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <f>(B11-$F$2)*($C$2-$C$3)/($F$3-$F$2)+$C$3</f>
+        <f t="shared" si="0"/>
         <v>56173</v>
       </c>
     </row>
@@ -953,7 +942,7 @@
         <v>4</v>
       </c>
       <c r="C12">
-        <f>(B12-$F$2)*($C$2-$C$3)/($F$3-$F$2)+$C$3</f>
+        <f t="shared" si="0"/>
         <v>51492</v>
       </c>
     </row>
@@ -962,7 +951,7 @@
         <v>3</v>
       </c>
       <c r="C13">
-        <f>(B13-$F$2)*($C$2-$C$3)/($F$3-$F$2)+$C$3</f>
+        <f t="shared" si="0"/>
         <v>46811</v>
       </c>
     </row>
@@ -971,7 +960,7 @@
         <v>2</v>
       </c>
       <c r="C14">
-        <f>(B14-$F$2)*($C$2-$C$3)/($F$3-$F$2)+$C$3</f>
+        <f t="shared" si="0"/>
         <v>42130</v>
       </c>
     </row>
@@ -980,7 +969,7 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <f>(B15-$F$2)*($C$2-$C$3)/($F$3-$F$2)+$C$3</f>
+        <f t="shared" si="0"/>
         <v>37449</v>
       </c>
     </row>
@@ -989,7 +978,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <f>(B16-$F$2)*($C$2-$C$3)/($F$3-$F$2)+$C$3</f>
+        <f t="shared" si="0"/>
         <v>32768</v>
       </c>
     </row>
@@ -998,7 +987,7 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <f>(B17-$F$4)*($C$4-$C$5)/($F$5-$F$4)+$C$5</f>
+        <f t="shared" ref="C17:C24" si="1">(B17-$F$4)*($C$4-$C$5)/($F$5-$F$4)+$C$5</f>
         <v>32767</v>
       </c>
     </row>
@@ -1007,7 +996,7 @@
         <v>14</v>
       </c>
       <c r="C18">
-        <f>(B18-$F$4)*($C$4-$C$5)/($F$5-$F$4)+$C$5</f>
+        <f t="shared" si="1"/>
         <v>28086</v>
       </c>
     </row>
@@ -1016,7 +1005,7 @@
         <v>13</v>
       </c>
       <c r="C19">
-        <f>(B19-$F$4)*($C$4-$C$5)/($F$5-$F$4)+$C$5</f>
+        <f t="shared" si="1"/>
         <v>23405</v>
       </c>
     </row>
@@ -1025,7 +1014,7 @@
         <v>12</v>
       </c>
       <c r="C20">
-        <f>(B20-$F$4)*($C$4-$C$5)/($F$5-$F$4)+$C$5</f>
+        <f t="shared" si="1"/>
         <v>18724</v>
       </c>
     </row>
@@ -1034,7 +1023,7 @@
         <v>11</v>
       </c>
       <c r="C21">
-        <f>(B21-$F$4)*($C$4-$C$5)/($F$5-$F$4)+$C$5</f>
+        <f t="shared" si="1"/>
         <v>14043</v>
       </c>
     </row>
@@ -1043,7 +1032,7 @@
         <v>10</v>
       </c>
       <c r="C22">
-        <f>(B22-$F$4)*($C$4-$C$5)/($F$5-$F$4)+$C$5</f>
+        <f t="shared" si="1"/>
         <v>9362</v>
       </c>
     </row>
@@ -1052,7 +1041,7 @@
         <v>9</v>
       </c>
       <c r="C23">
-        <f>(B23-$F$4)*($C$4-$C$5)/($F$5-$F$4)+$C$5</f>
+        <f t="shared" si="1"/>
         <v>4681</v>
       </c>
     </row>
@@ -1061,7 +1050,7 @@
         <v>8</v>
       </c>
       <c r="C24">
-        <f>(B24-$F$4)*($C$4-$C$5)/($F$5-$F$4)+$C$5</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>